<commit_message>
Made Charts Pretty in 2009
</commit_message>
<xml_diff>
--- a/2009Data/EnergyProfileCharts/EndConsumptionTable.xlsx
+++ b/2009Data/EnergyProfileCharts/EndConsumptionTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1080" windowWidth="22060" windowHeight="13680" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="60" windowWidth="22060" windowHeight="13680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Energy</t>
   </si>
@@ -73,13 +73,16 @@
   </si>
   <si>
     <t>Motor gas</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +121,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,23 +156,91 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F23" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F23"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Energy" dataDxfId="5"/>
+    <tableColumn id="2" name="Column1"/>
+    <tableColumn id="3" name="AZ" dataDxfId="4"/>
+    <tableColumn id="4" name="CA" dataDxfId="3"/>
+    <tableColumn id="5" name="NM" dataDxfId="2"/>
+    <tableColumn id="6" name="TX" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,34 +568,37 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -532,29 +618,29 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2"/>
+      <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <f>C2/C2</f>
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:F3" si="0">D2/D2</f>
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -574,29 +660,29 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f>C4/C2</f>
         <v>0.28416150248513089</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" ref="D5:F5" si="1">D4/D2</f>
         <v>6.5458804250802596E-3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f t="shared" si="1"/>
         <v>0.45689278436025732</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f t="shared" si="1"/>
         <v>0.13258395145216939</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -616,29 +702,29 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>C6/C2</f>
         <v>7.4933799678069013E-2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" ref="D7:F7" si="2">D6/D2</f>
         <v>0.19493983988545024</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f t="shared" si="2"/>
         <v>0.26128998964273592</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <f t="shared" si="2"/>
         <v>0.18113481666275183</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -658,29 +744,29 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f>C8/C2</f>
         <v>0.22817578058358004</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" ref="D9:F9" si="3">D8/D2</f>
         <v>0.23315710368706655</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f t="shared" si="3"/>
         <v>0.18024390499963724</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <f t="shared" si="3"/>
         <v>0.13369181528301435</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -700,29 +786,29 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>C10/C2</f>
         <v>9.8584553376232828E-2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" ref="D11:F11" si="4">D10/D2</f>
         <v>6.5787842048041334E-2</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f t="shared" si="4"/>
         <v>0.11118704210731102</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <f t="shared" si="4"/>
         <v>6.8133809497640432E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -742,29 +828,29 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f>C12/C2</f>
         <v>2.2201740997740978E-2</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <f t="shared" ref="D13:F13" si="5">D12/D2</f>
         <v>6.9399149425239864E-2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f t="shared" si="5"/>
         <v>1.1322697859899443E-2</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <f t="shared" si="5"/>
         <v>3.1020456077655051E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -784,29 +870,29 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2"/>
+      <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>C14/C2</f>
         <v>5.0322907086280478E-3</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" ref="D15:F15" si="6">D14/D2</f>
         <v>7.6115608014676699E-3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f t="shared" si="6"/>
         <v>3.3835549162464541E-2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <f t="shared" si="6"/>
         <v>0.13181777110833931</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
@@ -826,29 +912,29 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="2"/>
+      <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f>C16/C2</f>
         <v>0</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" ref="D17:F17" si="7">D16/D2</f>
         <v>3.0311182484248973E-2</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f t="shared" si="7"/>
         <v>9.3620901450953408E-5</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f t="shared" si="7"/>
         <v>1.3505313267641865E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B18" t="s">
@@ -868,29 +954,29 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <f>C18/C2</f>
         <v>1.4924662322491589E-3</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <f t="shared" ref="D19:F19" si="8">D18/D2</f>
         <v>2.7944298380182295E-2</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <f t="shared" si="8"/>
         <v>2.0584383004906101E-2</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f t="shared" si="8"/>
         <v>0.10064846249153628</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
@@ -910,29 +996,29 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
+      <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f>C20/C2</f>
         <v>2.4350191307129454E-2</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <f t="shared" ref="D21:F21" si="9">D20/D2</f>
         <v>2.8063493777470729E-2</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <f t="shared" si="9"/>
         <v>2.5810109482773791E-2</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <f t="shared" si="9"/>
         <v>1.312368660023485E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
@@ -952,33 +1038,37 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1"/>
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f>C22/C2</f>
         <v>2.2629138034151861E-4</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <f t="shared" ref="D23:F23" si="10">D22/D2</f>
         <v>2.5207125817173863E-4</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <f t="shared" si="10"/>
         <v>4.7316732734794739E-4</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <f t="shared" si="10"/>
         <v>1.8207941128699329E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="2"/>
+      <c r="A26" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>